<commit_message>
Added updateORCreate to import
</commit_message>
<xml_diff>
--- a/storage/importer/trails/EUMA_TRAILS_IMPORT_FILE_EXAMPLE.xlsx
+++ b/storage/importer/trails/EUMA_TRAILS_IMPORT_FILE_EXAMPLE.xlsx
@@ -9,14 +9,17 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7miWfXUgrxAUe3yFXOkD670tZs1Wyg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mi21cYecwzFQXwCy5mgotbOUlxqow=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+  <si>
+    <t>id</t>
+  </si>
   <si>
     <t>name</t>
   </si>
@@ -36,7 +39,7 @@
     <t>member_acronym</t>
   </si>
   <si>
-    <t>Percorso N35</t>
+    <t>1</t>
   </si>
   <si>
     <t>N35</t>
@@ -51,7 +54,7 @@
     <t>CAI</t>
   </si>
   <si>
-    <t>Percorso 218</t>
+    <t>2</t>
   </si>
   <si>
     <t>218</t>
@@ -63,7 +66,7 @@
     <t>https://osm2cai.cai.it/api/v1/hiking-route/18818</t>
   </si>
   <si>
-    <t>Percorso 648</t>
+    <t>3</t>
   </si>
   <si>
     <t>648</t>
@@ -75,7 +78,7 @@
     <t>https://osm2cai.cai.it/api/v1/hiking-route/6879</t>
   </si>
   <si>
-    <t>Percorso 542</t>
+    <t>4</t>
   </si>
   <si>
     <t>542</t>
@@ -87,7 +90,7 @@
     <t>https://osm2cai.cai.it/api/v1/hiking-route/4993</t>
   </si>
   <si>
-    <t>Percorso E01A</t>
+    <t>5</t>
   </si>
   <si>
     <t>E01A</t>
@@ -103,7 +106,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -129,10 +132,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -140,7 +139,7 @@
     <font>
       <u/>
       <sz val="10.0"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -180,15 +179,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
@@ -200,24 +199,21 @@
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -437,13 +433,15 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="43.29"/>
-    <col customWidth="1" min="2" max="3" width="21.86"/>
-    <col customWidth="1" min="4" max="4" width="20.86"/>
-    <col customWidth="1" min="5" max="5" width="22.14"/>
-    <col customWidth="1" min="6" max="6" width="29.0"/>
-    <col customWidth="1" min="7" max="7" width="29.57"/>
-    <col customWidth="1" min="8" max="15" width="8.71"/>
+    <col customWidth="1" min="1" max="1" width="9.86"/>
+    <col customWidth="1" min="2" max="2" width="10.43"/>
+    <col customWidth="1" min="3" max="3" width="8.86"/>
+    <col customWidth="1" min="4" max="4" width="41.43"/>
+    <col customWidth="1" min="5" max="5" width="18.71"/>
+    <col customWidth="1" min="6" max="6" width="47.57"/>
+    <col customWidth="1" min="7" max="7" width="29.0"/>
+    <col customWidth="1" min="8" max="8" width="29.57"/>
+    <col customWidth="1" min="9" max="16" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="21.75" customHeight="1">
@@ -453,20 +451,22 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="6"/>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -474,154 +474,160 @@
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
     </row>
     <row r="2" ht="26.25" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="E2" s="9"/>
+      <c r="F2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
+      <c r="G2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="12"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
     </row>
     <row r="3" ht="21.0" customHeight="1">
       <c r="A3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11" t="s">
+      <c r="D4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
     </row>
     <row r="5" ht="16.5" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="11" t="s">
+      <c r="D5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="13"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="12"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
     </row>
     <row r="6" ht="16.5" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11" t="s">
+      <c r="D6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="13"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="12"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C2"/>
-    <hyperlink r:id="rId2" ref="E2"/>
-    <hyperlink r:id="rId3" ref="C3"/>
-    <hyperlink r:id="rId4" ref="E3"/>
-    <hyperlink r:id="rId5" ref="C4"/>
-    <hyperlink r:id="rId6" ref="E4"/>
-    <hyperlink r:id="rId7" ref="C5"/>
-    <hyperlink r:id="rId8" ref="E5"/>
-    <hyperlink r:id="rId9" ref="C6"/>
-    <hyperlink r:id="rId10" ref="E6"/>
+    <hyperlink r:id="rId1" ref="D2"/>
+    <hyperlink r:id="rId2" ref="F2"/>
+    <hyperlink r:id="rId3" ref="D3"/>
+    <hyperlink r:id="rId4" ref="F3"/>
+    <hyperlink r:id="rId5" ref="D4"/>
+    <hyperlink r:id="rId6" ref="F4"/>
+    <hyperlink r:id="rId7" ref="D5"/>
+    <hyperlink r:id="rId8" ref="F5"/>
+    <hyperlink r:id="rId9" ref="D6"/>
+    <hyperlink r:id="rId10" ref="F6"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.15748031496062992" footer="0.0" header="0.0" left="0.11811023622047245" right="0.11811023622047245" top="1.5208333333333333"/>

</xml_diff>